<commit_message>
ran sporangia models for both conifers and broadleaf assays togehter in same script. updated with good priors and standardized the units of the posteriors. have nice looking plots and model outputs saved.
</commit_message>
<xml_diff>
--- a/data2019/master_bothassays.xlsx
+++ b/data2019/master_bothassays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarosenthal/Box/Competency project/competency.git/data2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3405A5C-7488-7147-948D-FD2E22798BD2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8449F8A1-AE18-9449-AB96-3F763AF9C6D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="-4020" windowWidth="25600" windowHeight="20000" xr2:uid="{A76F92BD-BCFB-5343-B244-DAB25E6FE268}"/>
   </bookViews>
@@ -4363,11 +4363,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCE57EC-029C-1045-9B03-14F4EFD065BE}">
-  <dimension ref="A1:V1201"/>
+  <dimension ref="A1:T1201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <pane ySplit="1" topLeftCell="A882" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X1075" sqref="X1075"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -60186,7 +60186,7 @@
         <v>0.65582041165113869</v>
       </c>
     </row>
-    <row r="1073" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1073" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1073" s="10">
         <v>632</v>
       </c>
@@ -60233,7 +60233,7 @@
         <v>0.44076448879677388</v>
       </c>
     </row>
-    <row r="1074" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1074" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1074" s="10">
         <v>633</v>
       </c>
@@ -60280,7 +60280,7 @@
         <v>0.61102468174243951</v>
       </c>
     </row>
-    <row r="1075" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1075" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1075" s="10">
         <v>633</v>
       </c>
@@ -60327,7 +60327,7 @@
         <v>0.58216239235004597</v>
       </c>
     </row>
-    <row r="1076" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1076" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1076" s="10">
         <v>634</v>
       </c>
@@ -60374,7 +60374,7 @@
         <v>0.71481966567723032</v>
       </c>
     </row>
-    <row r="1077" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1077" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1077" s="10">
         <v>634</v>
       </c>
@@ -60421,7 +60421,7 @@
         <v>0.6732106238717922</v>
       </c>
     </row>
-    <row r="1078" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1078" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1078" s="10">
         <v>635</v>
       </c>
@@ -60468,7 +60468,7 @@
         <v>0.4695357299576457</v>
       </c>
     </row>
-    <row r="1079" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1079" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1079" s="10">
         <v>635</v>
       </c>
@@ -60515,7 +60515,7 @@
         <v>0.34844158203372311</v>
       </c>
     </row>
-    <row r="1080" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1080" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1080" s="10">
         <v>636</v>
       </c>
@@ -60556,13 +60556,14 @@
         <v>1260</v>
       </c>
       <c r="P1080">
-        <v>103.63733618614603</v>
+        <v>72.757731958762889</v>
       </c>
       <c r="Q1080">
-        <v>0.34042933765980943</v>
-      </c>
-    </row>
-    <row r="1081" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0.5294986018223341</v>
+      </c>
+      <c r="S1080"/>
+    </row>
+    <row r="1081" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1081" s="10">
         <v>636</v>
       </c>
@@ -60603,13 +60604,14 @@
         <v>1</v>
       </c>
       <c r="P1081">
-        <v>77.205882352941174</v>
+        <v>40.845528455284551</v>
       </c>
       <c r="Q1081">
-        <v>0.81724892613919486</v>
-      </c>
-    </row>
-    <row r="1082" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0.55952171842050769</v>
+      </c>
+      <c r="S1081"/>
+    </row>
+    <row r="1082" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1082" s="10">
         <v>637</v>
       </c>
@@ -60656,7 +60658,7 @@
         <v>0.34953416081198407</v>
       </c>
     </row>
-    <row r="1083" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1083" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1083" s="10">
         <v>637</v>
       </c>
@@ -60703,7 +60705,7 @@
         <v>0.32595266884785179</v>
       </c>
     </row>
-    <row r="1084" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1084" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1084" s="10">
         <v>638</v>
       </c>
@@ -60750,7 +60752,7 @@
         <v>0.54656253382504305</v>
       </c>
     </row>
-    <row r="1085" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1085" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1085" s="10">
         <v>638</v>
       </c>
@@ -60797,7 +60799,7 @@
         <v>0.61020524765874373</v>
       </c>
     </row>
-    <row r="1086" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1086" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1086" s="10">
         <v>639</v>
       </c>
@@ -60844,7 +60846,7 @@
         <v>0.57114555633591457</v>
       </c>
     </row>
-    <row r="1087" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1087" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1087" s="10">
         <v>639</v>
       </c>
@@ -60891,7 +60893,7 @@
         <v>0.51369412224569266</v>
       </c>
     </row>
-    <row r="1088" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1088" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1088" s="10">
         <v>640</v>
       </c>

</xml_diff>